<commit_message>
Correciones menores,trabajando en rellenado de multicelda
</commit_message>
<xml_diff>
--- a/manto_feeder.xlsx
+++ b/manto_feeder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_oneasg_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/mantto_feeder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_BA7CC89E462F7C7754BEDAF2CE622075F44318BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76211A5B-5147-40C4-8906-5EAEFD1A3E74}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_BA7CC89E462F7C7754BEDAF2CE622075F44318BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E3E55C0-FEDB-4A10-B2A5-FD33AB2B86BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nombre</t>
   </si>
@@ -31,13 +31,13 @@
     <t>datos fusionados</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>Cristian</t>
   </si>
   <si>
     <t>Echevarria</t>
+  </si>
+  <si>
+    <t>DATOS FUSIONADOS</t>
   </si>
 </sst>
 </file>
@@ -371,13 +371,13 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -391,91 +391,81 @@
         <v>2</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
trabajando en script para relleno de celdas,y localizacion de ID
</commit_message>
<xml_diff>
--- a/manto_feeder.xlsx
+++ b/manto_feeder.xlsx
@@ -1,66 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_oneasg_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/mantto_feeder/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_BA7CC89E462F7C7754BEDAF2CE622075F44318BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E3E55C0-FEDB-4A10-B2A5-FD33AB2B86BF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>datos fusionados</t>
-  </si>
-  <si>
-    <t>Cristian</t>
-  </si>
-  <si>
-    <t>Echevarria</t>
-  </si>
-  <si>
-    <t>DATOS FUSIONADOS</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Arial"/>
+      <b val="1"/>
       <sz val="20"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,32 +48,91 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -367,114 +398,239 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="3" width="20"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="3" width="17.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+    <row customHeight="1" ht="26.25" r="1" s="3">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Apellido</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>datos fusionados</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cristian</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Echevarria</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>23760055</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A10:F17"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K0000FF_x000D_# This data is internal to Brunswick._x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0000FF This data is internal to Brunswick.</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K0000FF_x000d_# This data is internal to Brunswick._x000d_&amp;1#&amp;"Calibri"&amp;10 &amp;K0000FF This data is internal to Brunswick.</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
issue resuelto,ya se puede rellanar rango de columnas y se deteiene el proceso si se encuentra una celda con datos
</commit_message>
<xml_diff>
--- a/manto_feeder.xlsx
+++ b/manto_feeder.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="7200" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,12 +54,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -403,19 +403,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="20"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="3" width="17.5703125"/>
+    <col customWidth="1" max="1" min="1" style="4" width="20"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="17.5703125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26.25" r="1" s="3">
+    <row customHeight="1" ht="26.25" r="1" s="4">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nombre</t>
@@ -426,9 +426,74 @@
           <t>Apellido</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>datos fusionados</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -444,18 +509,50 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
+    <row r="3">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+    </row>
     <row r="4"/>
     <row r="5">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="2" t="n">
         <v>23760055</v>
       </c>
+      <c r="B5" t="n">
+        <v>23760055</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>valor</t>
-        </is>
+      <c r="A6" t="n">
+        <v>23760055</v>
       </c>
     </row>
     <row r="7"/>
@@ -466,17 +563,142 @@
     <row r="12"/>
     <row r="13"/>
     <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
+    <row r="15">
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -508,111 +730,6 @@
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>